<commit_message>
Delete Row Admin module
</commit_message>
<xml_diff>
--- a/src/database/Showtime.xlsx
+++ b/src/database/Showtime.xlsx
@@ -460,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA69B54E-1050-4942-9338-6C6E0043CE56}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -591,23 +591,6 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>